<commit_message>
Change PAC sheet name
</commit_message>
<xml_diff>
--- a/Shiny-PAC/PAC_config.xlsx
+++ b/Shiny-PAC/PAC_config.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/sandlin_cole_epa_gov/Documents/Profile/Documents/GitHub/Water_Treatment_Models/Shiny-PAC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="302" documentId="8_{FC6C552E-3166-4C64-8BC2-E954C229B3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D29DCF02-F9AF-49D5-955E-D3D9BF09F505}"/>
+  <xr:revisionPtr revIDLastSave="303" documentId="8_{FC6C552E-3166-4C64-8BC2-E954C229B3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC49C721-43B0-4D2F-A346-4693F12FBE59}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{317BF3F6-A68C-4964-9BC3-AEDC7E3058F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Contactor" sheetId="4" r:id="rId1"/>
-    <sheet name="PAC" sheetId="10" r:id="rId2"/>
+    <sheet name="PAC Characteristics" sheetId="10" r:id="rId2"/>
     <sheet name="Compounds" sheetId="1" r:id="rId3"/>
     <sheet name="name" sheetId="11" r:id="rId4"/>
   </sheets>
@@ -244,6 +244,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>